<commit_message>
cambios db, marco avances de programacion, y subo nuevo DER
</commit_message>
<xml_diff>
--- a/Producto/04-It_I/01-Requerimientos/DiseñoGráfico/trash.pantallas.checklist.xlsx
+++ b/Producto/04-It_I/01-Requerimientos/DiseñoGráfico/trash.pantallas.checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>actualizar_domicilio.png</t>
   </si>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -478,6 +478,9 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
       <c r="C3" t="s">
         <v>33</v>
       </c>
@@ -501,6 +504,9 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
@@ -566,6 +572,9 @@
       <c r="A17" t="s">
         <v>15</v>
       </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
       <c r="C17" t="s">
         <v>33</v>
       </c>
@@ -605,15 +614,33 @@
       <c r="A23" t="s">
         <v>21</v>
       </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3">

</xml_diff>